<commit_message>
Added some entries to Timesheet.xlsx
</commit_message>
<xml_diff>
--- a/.idea/project-admin/Timesheet.xlsx
+++ b/.idea/project-admin/Timesheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mclaw\IdeaProjects\COSC2626-A1\.idea\project-admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8F3D88-CE12-4ABB-BB7E-D90829BF7875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033910C2-28D2-4898-8039-74615167B95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="2832" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bob Timesheet" sheetId="5" r:id="rId1"/>
-    <sheet name="Marty Timesheet" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="Bob Timesheet" sheetId="5" r:id="rId2"/>
+    <sheet name="Marty Timesheet" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Week</t>
   </si>
@@ -55,6 +56,39 @@
   </si>
   <si>
     <t>Activity</t>
+  </si>
+  <si>
+    <t>Worked on W3-S3-Tasks - research of how to download objects via x-byte chunks</t>
+  </si>
+  <si>
+    <t>Created GitHub repo for collab and added scripts + data. Also created project timesheet.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please make sure that you edit/view save this file via Excel and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> IntelliJ built-in editor. Failure to do so may cause the formatting/formulas to be damaged, as the built-in editor seems to want to treat this file as *.csv.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -82,15 +116,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -209,11 +249,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -229,6 +349,36 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,13 +501,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -368,6 +511,13 @@
           <color indexed="64"/>
         </top>
         <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -401,6 +551,144 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -428,144 +716,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -580,30 +730,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECD6CB37-26DE-4072-9B09-DDD5FBB95AA2}" name="Table13" displayName="Table13" ref="A1:F10" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECD6CB37-26DE-4072-9B09-DDD5FBB95AA2}" name="Table13" displayName="Table13" ref="A1:F10" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:F10" xr:uid="{ECD6CB37-26DE-4072-9B09-DDD5FBB95AA2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0887FFD3-0D2C-483A-A87E-C17D140D46E4}" name="Week" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1BF21DB7-9577-4A0D-B1F7-548AEC6443CC}" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{164B6E99-4AF1-4B16-9127-F40C08228600}" name="Time in" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{0CEE4F58-5E6E-4654-BFDC-B4CEF5D1D385}" name="Time out" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{0D40069E-9353-4945-88F4-FC7551A72377}" name="Duration(hour)" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{981468CE-B740-4CA2-AE39-58CCAF12D0D1}" name="Activity" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0887FFD3-0D2C-483A-A87E-C17D140D46E4}" name="Week" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1BF21DB7-9577-4A0D-B1F7-548AEC6443CC}" name="Date" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{164B6E99-4AF1-4B16-9127-F40C08228600}" name="Time in" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{0CEE4F58-5E6E-4654-BFDC-B4CEF5D1D385}" name="Time out" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{0D40069E-9353-4945-88F4-FC7551A72377}" name="Duration(hour)" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{981468CE-B740-4CA2-AE39-58CCAF12D0D1}" name="Activity" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A526B132-D9B2-41FA-91FD-6E0BD9C6D47C}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
-  <autoFilter ref="A1:F10" xr:uid="{A526B132-D9B2-41FA-91FD-6E0BD9C6D47C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A526B132-D9B2-41FA-91FD-6E0BD9C6D47C}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F11" xr:uid="{A526B132-D9B2-41FA-91FD-6E0BD9C6D47C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9F59873D-EE4B-429B-B89C-A87828E7ABF9}" name="Week" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{D21402AF-8D68-4A63-B80C-46BF7C71FEEF}" name="Date" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{27CAD598-B04A-4A83-A745-22043EA69FB0}" name="Time in" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{5437ECC6-A7A1-453A-813A-B49331733E27}" name="Time out" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{D958AEE7-8C16-4237-A980-337C1DF08C2D}" name="Duration(hour)" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{C6E7C0D9-44C1-4F8E-B57C-FB8E6E43E744}" name="Activity" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{9F59873D-EE4B-429B-B89C-A87828E7ABF9}" name="Week" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{D21402AF-8D68-4A63-B80C-46BF7C71FEEF}" name="Date" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{27CAD598-B04A-4A83-A745-22043EA69FB0}" name="Time in" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{5437ECC6-A7A1-453A-813A-B49331733E27}" name="Time out" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D958AEE7-8C16-4237-A980-337C1DF08C2D}" name="Duration(hour)" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C6E7C0D9-44C1-4F8E-B57C-FB8E6E43E744}" name="Activity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -925,6 +1075,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D0ACB-7638-4870-BAF6-93E97F620E77}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B22C6F-7E95-46FA-83D6-F011AE9E7662}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -938,7 +1207,7 @@
     <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1078,12 +1347,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAAD7A6-5C47-4348-9B1A-A80A9436C714}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,7 +1361,7 @@
     <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1119,110 +1388,139 @@
       <c r="A2" s="5">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="2">
+        <v>45734</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="E2" s="4">
         <f>D2-C2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="6"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="5">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45735</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.90625</v>
+      </c>
       <c r="E3" s="4">
-        <f>SUM(E2:E2)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="6"/>
+        <f>Table1[[#This Row],[Time out]]-Table1[[#This Row],[Time in]]</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>4</v>
-      </c>
+      <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4">
-        <f>D4-C4</f>
-        <v>0</v>
+        <f>SUM(E2:E3)</f>
+        <v>0.11458333333333337</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4">
-        <f>SUM(E4:E4)</f>
+        <f>D5-C5</f>
         <v>0</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
+      <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4">
-        <f>D6-C6</f>
+        <f>SUM(E5:E5)</f>
         <v>0</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4">
-        <f>SUM(E6:E6)</f>
+        <f>D7-C7</f>
         <v>0</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
+      <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4">
-        <f>D8-C8</f>
+        <f>SUM(E7:E7)</f>
         <v>0</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5">
+        <v>6</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4">
-        <f>SUM(E6:E8)</f>
+        <f>D9-C9</f>
         <v>0</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4">
+        <f>SUM(E7:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>7</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13">
-        <f t="shared" ref="E10" si="0">D10-C10</f>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13">
+        <f t="shared" ref="E11" si="0">D11-C11</f>
         <v>0</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F11" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1233,6 +1531,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dcbdea14-a3c4-43d2-81af-a36cd4e9f139" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="04d16460-b646-41f0-8934-05fac8b8aa37">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A46513FC5C9DBD4B8E8F12E4BEC953F6" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="79447f7872eec1c6c03a755451af2d41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04d16460-b646-41f0-8934-05fac8b8aa37" xmlns:ns3="dcbdea14-a3c4-43d2-81af-a36cd4e9f139" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7049ecd096509e15af6fa5b74dae3f08" ns2:_="" ns3:_="">
     <xsd:import namespace="04d16460-b646-41f0-8934-05fac8b8aa37"/>
@@ -1467,27 +1785,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dcbdea14-a3c4-43d2-81af-a36cd4e9f139" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="04d16460-b646-41f0-8934-05fac8b8aa37">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6A70F24-1D55-488B-B3A0-428DB2594092}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D505DD8-1EEF-4322-B25A-FB4B43DB09E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dcbdea14-a3c4-43d2-81af-a36cd4e9f139"/>
+    <ds:schemaRef ds:uri="04d16460-b646-41f0-8934-05fac8b8aa37"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDBAA53F-E5A1-491A-B3DC-C86AC4A022C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1504,23 +1821,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D505DD8-1EEF-4322-B25A-FB4B43DB09E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dcbdea14-a3c4-43d2-81af-a36cd4e9f139"/>
-    <ds:schemaRef ds:uri="04d16460-b646-41f0-8934-05fac8b8aa37"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6A70F24-1D55-488B-B3A0-428DB2594092}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Timesheet-README.md and edited main README.md
</commit_message>
<xml_diff>
--- a/.idea/project-admin/Timesheet.xlsx
+++ b/.idea/project-admin/Timesheet.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mclaw\IdeaProjects\COSC2626-A1\.idea\project-admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033910C2-28D2-4898-8039-74615167B95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD91535-A780-436D-8F44-1E067C420C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
-    <sheet name="Bob Timesheet" sheetId="5" r:id="rId2"/>
-    <sheet name="Marty Timesheet" sheetId="4" r:id="rId3"/>
+    <sheet name="Bob Timesheet" sheetId="5" r:id="rId1"/>
+    <sheet name="Marty Timesheet" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Week</t>
   </si>
@@ -62,33 +61,6 @@
   </si>
   <si>
     <t>Created GitHub repo for collab and added scripts + data. Also created project timesheet.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Please make sure that you edit/view save this file via Excel and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>not</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> IntelliJ built-in editor. Failure to do so may cause the formatting/formulas to be damaged, as the built-in editor seems to want to treat this file as *.csv.</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -116,21 +88,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -249,91 +215,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -349,36 +235,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,130 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D0ACB-7638-4870-BAF6-93E97F620E77}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B22C6F-7E95-46FA-83D6-F011AE9E7662}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,7 +1084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAAD7A6-5C47-4348-9B1A-A80A9436C714}">
   <dimension ref="A1:F11"/>
   <sheetViews>

</xml_diff>